<commit_message>
updated scrumfile, channged datahander package
</commit_message>
<xml_diff>
--- a/Documentation/Scrum.xlsx
+++ b/Documentation/Scrum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -17,10 +17,12 @@
     <sheet name="20.04" sheetId="5" r:id="rId3"/>
     <sheet name="22.04" sheetId="4" r:id="rId4"/>
     <sheet name="24.04" sheetId="7" r:id="rId5"/>
+    <sheet name="26.04" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'22.04'!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'24.04'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'26.04'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="55">
   <si>
     <t>Actual remaining hours</t>
   </si>
@@ -73,9 +75,6 @@
     <t>Façade design pattern</t>
   </si>
   <si>
-    <t>Adapter design pattern</t>
-  </si>
-  <si>
     <t>Remote observer d.p.</t>
   </si>
   <si>
@@ -142,18 +141,9 @@
     <t>Create client GUI</t>
   </si>
   <si>
-    <t>Implement façade design pattern</t>
-  </si>
-  <si>
     <t xml:space="preserve">Document façade </t>
   </si>
   <si>
-    <t>In progress</t>
-  </si>
-  <si>
-    <t>Documentation of Client-Server</t>
-  </si>
-  <si>
     <t>Krzysztof</t>
   </si>
   <si>
@@ -169,10 +159,46 @@
     <t>Marek, Stela</t>
   </si>
   <si>
-    <t xml:space="preserve">Implement proxy design pattern </t>
-  </si>
-  <si>
     <t>Andreea</t>
+  </si>
+  <si>
+    <t>Start documentation of Client-Server</t>
+  </si>
+  <si>
+    <t>After connecting client to server, current trip list is displayed</t>
+  </si>
+  <si>
+    <t>Show current trip list</t>
+  </si>
+  <si>
+    <t>Implement displaying trip list</t>
+  </si>
+  <si>
+    <t>Marek</t>
+  </si>
+  <si>
+    <t>Customer wants iterator design pattern</t>
+  </si>
+  <si>
+    <t>Proxy design pattern</t>
+  </si>
+  <si>
+    <t>Iterator design pattern</t>
+  </si>
+  <si>
+    <t>Implement iterator design pattern</t>
+  </si>
+  <si>
+    <t>Document iterator</t>
+  </si>
+  <si>
+    <t>Implement proxy design pattern</t>
+  </si>
+  <si>
+    <t>Document proxy</t>
+  </si>
+  <si>
+    <t>Started</t>
   </si>
 </sst>
 </file>
@@ -380,7 +406,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$A$10</c:f>
+              <c:f>'Burndown Chart'!$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -444,36 +470,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$10:$J$10</c:f>
+              <c:f>'Burndown Chart'!$B$12:$J$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>57</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>55</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>55</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>55</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>55</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -490,7 +516,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$A$11</c:f>
+              <c:f>'Burndown Chart'!$A$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -554,33 +580,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$11:$J$11</c:f>
+              <c:f>'Burndown Chart'!$B$13:$J$13</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>57</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.875</c:v>
+                  <c:v>55.125</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42.75</c:v>
+                  <c:v>47.25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>35.625</c:v>
+                  <c:v>39.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.5</c:v>
+                  <c:v>31.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.375</c:v>
+                  <c:v>23.625</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14.25</c:v>
+                  <c:v>15.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.125</c:v>
+                  <c:v>7.875</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
                   <c:v>0</c:v>
@@ -1340,13 +1366,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>857249</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1672,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,10 +1774,10 @@
     </row>
     <row r="3" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B3" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
@@ -1762,16 +1788,16 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="5">
-        <f t="shared" ref="K3:K7" si="0">SUM(C3:J3)</f>
+        <f t="shared" ref="K3:K9" si="0">SUM(C3:J3)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
@@ -1788,10 +1814,10 @@
     </row>
     <row r="5" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1808,14 +1834,17 @@
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="B6" s="5">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="E6" s="6">
+        <f>B6</f>
+        <v>3</v>
+      </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
@@ -1823,15 +1852,15 @@
       <c r="J6" s="6"/>
       <c r="K6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="B7" s="5">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1848,15 +1877,13 @@
     </row>
     <row r="8" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="6">
-        <v>2</v>
-      </c>
+      <c r="D8" s="6"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1864,97 +1891,139 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="5">
-        <f>SUM(C8:J8)</f>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="5">
+        <v>3</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="K9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="5">
+        <f t="shared" ref="K3:K10" si="1">SUM(C10:J10)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="5">
-        <f>SUM(B2:B8)</f>
-        <v>57</v>
-      </c>
-      <c r="C10" s="5">
-        <f>B10-(SUM(C2:C8))</f>
-        <v>57</v>
-      </c>
-      <c r="D10" s="5">
-        <f t="shared" ref="D10:J10" si="1">C10-(SUM(D2:D8))</f>
-        <v>55</v>
-      </c>
-      <c r="E10" s="5">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="F10" s="5">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="G10" s="5">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="H10" s="5">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="I10" s="5">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-      <c r="J10" s="5">
-        <f t="shared" si="1"/>
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B12" s="5">
+        <f>SUM(B2:B10)</f>
+        <v>63</v>
+      </c>
+      <c r="C12" s="5">
+        <f>B12-(SUM(C2:C10))</f>
+        <v>63</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" ref="D12:J12" si="2">C12-(SUM(D2:D10))</f>
+        <v>61</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="H12" s="5">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="I12" s="5">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="J12" s="5">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="5">
-        <f>SUM(B2:B8)</f>
-        <v>57</v>
-      </c>
-      <c r="C11" s="7">
-        <f>B11-($B$11/8)</f>
-        <v>49.875</v>
-      </c>
-      <c r="D11" s="7">
-        <f t="shared" ref="D11:I11" si="2">C11-($B$11/8)</f>
-        <v>42.75</v>
-      </c>
-      <c r="E11" s="7">
-        <f t="shared" si="2"/>
-        <v>35.625</v>
-      </c>
-      <c r="F11" s="7">
-        <f t="shared" si="2"/>
-        <v>28.5</v>
-      </c>
-      <c r="G11" s="7">
-        <f t="shared" si="2"/>
-        <v>21.375</v>
-      </c>
-      <c r="H11" s="7">
-        <f t="shared" si="2"/>
-        <v>14.25</v>
-      </c>
-      <c r="I11" s="7">
-        <f t="shared" si="2"/>
-        <v>7.125</v>
-      </c>
-      <c r="J11" s="5">
-        <f>I11-($B$11/8)</f>
+      <c r="B13" s="5">
+        <f>SUM(B2:B10)</f>
+        <v>63</v>
+      </c>
+      <c r="C13" s="7">
+        <f>B13-($B$13/8)</f>
+        <v>55.125</v>
+      </c>
+      <c r="D13" s="7">
+        <f t="shared" ref="D13:I13" si="3">C13-($B$13/8)</f>
+        <v>47.25</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="3"/>
+        <v>39.375</v>
+      </c>
+      <c r="F13" s="7">
+        <f t="shared" si="3"/>
+        <v>31.5</v>
+      </c>
+      <c r="G13" s="7">
+        <f t="shared" si="3"/>
+        <v>23.625</v>
+      </c>
+      <c r="H13" s="7">
+        <f t="shared" si="3"/>
+        <v>15.75</v>
+      </c>
+      <c r="I13" s="7">
+        <f t="shared" si="3"/>
+        <v>7.875</v>
+      </c>
+      <c r="J13" s="5">
+        <f>I13-($B$13/8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:11" s="8" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:11" s="8" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1964,10 +2033,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1992,11 +2061,11 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A10" si="0">A2+1</f>
+        <f t="shared" ref="A3:A12" si="0">A2+1</f>
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C3">
         <f>'Burndown Chart'!B2</f>
@@ -2012,14 +2081,14 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <f>'Burndown Chart'!B3</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2028,14 +2097,14 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <f>'Burndown Chart'!B6</f>
-        <v>28</v>
+        <f>'Burndown Chart'!B4</f>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2044,14 +2113,14 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <f>'Burndown Chart'!B8</f>
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
-      </c>
-      <c r="C6">
-        <f>'Burndown Chart'!B5</f>
-        <v>7</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2060,14 +2129,14 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <f>'Burndown Chart'!B4</f>
-        <v>3</v>
+        <f>'Burndown Chart'!B7</f>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2076,14 +2145,14 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <f>'Burndown Chart'!B6/4</f>
-        <v>7</v>
+        <f>'Burndown Chart'!B6</f>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2092,14 +2161,14 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <f>'Burndown Chart'!B7</f>
+        <f>'Burndown Chart'!B5</f>
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2108,14 +2177,46 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <f>'Burndown Chart'!B8/4</f>
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <f>'Burndown Chart'!B9</f>
+        <v>3</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <f>'Burndown Chart'!B10</f>
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
         <v>33</v>
-      </c>
-      <c r="C10">
-        <f>'Burndown Chart'!B8</f>
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -2145,22 +2246,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -2173,7 +2274,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:F2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2188,22 +2289,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2214,16 +2315,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
         <v>26</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
       </c>
       <c r="E2">
         <v>0.5</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2234,16 +2335,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2254,36 +2355,36 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -2296,7 +2397,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2311,42 +2412,205 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
+        <v>7</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="2.85546875" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2357,96 +2621,36 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
         <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5">
-        <v>0.5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>4</v>
-      </c>
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated scrum, split some tasks...
</commit_message>
<xml_diff>
--- a/Documentation/Scrum.xlsx
+++ b/Documentation/Scrum.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="85">
   <si>
     <t>Actual remaining hours</t>
   </si>
@@ -228,9 +228,6 @@
     <t>Low</t>
   </si>
   <si>
-    <t>Customer require to test observer</t>
-  </si>
-  <si>
     <t>Customer wants singleton design pattern</t>
   </si>
   <si>
@@ -274,6 +271,27 @@
   </si>
   <si>
     <t>Implement showing trips in given date interval</t>
+  </si>
+  <si>
+    <t>Junit test for proxy</t>
+  </si>
+  <si>
+    <t>Customer require to test proxy</t>
+  </si>
+  <si>
+    <t>Junit test for proxy design pattern</t>
+  </si>
+  <si>
+    <t>Not started</t>
+  </si>
+  <si>
+    <t>Fix displaying trips in date interval in GUI</t>
+  </si>
+  <si>
+    <t>Finnish Client-Server documentation</t>
+  </si>
+  <si>
+    <t>Finnish MVC documentation</t>
   </si>
 </sst>
 </file>
@@ -481,7 +499,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$A$14</c:f>
+              <c:f>'Burndown Chart'!$A$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -542,7 +560,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$14:$I$14</c:f>
+              <c:f>'Burndown Chart'!$B$15:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -559,16 +577,16 @@
                   <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.5</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>25.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25.5</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -585,7 +603,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$A$15</c:f>
+              <c:f>'Burndown Chart'!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -646,7 +664,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$15:$I$15</c:f>
+              <c:f>'Burndown Chart'!$B$16:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1429,13 +1447,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>857249</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1761,10 +1779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,13 +1844,13 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="5">
-        <f t="shared" ref="J2:J12" si="0">SUM(C2:I2)</f>
+        <f t="shared" ref="J2:J13" si="0">SUM(C2:I2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
@@ -1919,20 +1937,20 @@
         <v>13</v>
       </c>
       <c r="B7" s="5">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6">
-        <v>16.5</v>
+        <v>18</v>
       </c>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="5">
         <f t="shared" si="0"/>
-        <v>16.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1977,7 +1995,7 @@
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" s="5">
         <v>3</v>
@@ -1996,7 +2014,7 @@
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="5">
         <v>5</v>
@@ -2017,7 +2035,7 @@
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B12" s="5">
         <v>3</v>
@@ -2037,84 +2055,103 @@
       </c>
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A13" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B13" s="5">
+        <v>4</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="5">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="B14" s="5">
-        <f>SUM(B2:B12)</f>
+    </row>
+    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="5">
+        <f>SUM(B2:B13)</f>
         <v>68</v>
       </c>
-      <c r="C14" s="5">
-        <f>B14-(SUM(C2:C12))</f>
+      <c r="C15" s="5">
+        <f>B15-(SUM(C2:C13))</f>
         <v>67</v>
       </c>
-      <c r="D14" s="5">
-        <f t="shared" ref="D14:I14" si="1">C14-(SUM(D2:D12))</f>
+      <c r="D15" s="5">
+        <f t="shared" ref="D15:I15" si="1">C15-(SUM(D2:D13))</f>
         <v>57</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E15" s="5">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F15" s="5">
         <f t="shared" si="1"/>
-        <v>28.5</v>
-      </c>
-      <c r="G14" s="5">
+        <v>27</v>
+      </c>
+      <c r="G15" s="5">
         <f t="shared" si="1"/>
-        <v>25.5</v>
-      </c>
-      <c r="H14" s="5">
+        <v>24</v>
+      </c>
+      <c r="H15" s="5">
         <f t="shared" si="1"/>
-        <v>25.5</v>
-      </c>
-      <c r="I14" s="5">
+        <v>24</v>
+      </c>
+      <c r="I15" s="5">
         <f t="shared" si="1"/>
-        <v>25.5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="5">
-        <f>SUM(B2:B12)</f>
+      <c r="B16" s="5">
+        <f>SUM(B2:B13)</f>
         <v>68</v>
       </c>
-      <c r="C15" s="7">
-        <f>B15-($B$15/7)</f>
+      <c r="C16" s="7">
+        <f>B16-($B$16/7)</f>
         <v>58.285714285714285</v>
       </c>
-      <c r="D15" s="7">
-        <f t="shared" ref="D15:I15" si="2">C15-($B$15/7)</f>
+      <c r="D16" s="7">
+        <f t="shared" ref="D16:I16" si="2">C16-($B$16/7)</f>
         <v>48.571428571428569</v>
       </c>
-      <c r="E15" s="7">
+      <c r="E16" s="7">
         <f t="shared" si="2"/>
         <v>38.857142857142854</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F16" s="7">
         <f t="shared" si="2"/>
         <v>29.142857142857139</v>
       </c>
-      <c r="G15" s="7">
+      <c r="G16" s="7">
         <f t="shared" si="2"/>
         <v>19.428571428571423</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H16" s="7">
         <f t="shared" si="2"/>
         <v>9.71428571428571</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I16" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="8" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" s="8" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2127,7 +2164,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2191,8 +2228,8 @@
         <v>15</v>
       </c>
       <c r="C5">
-        <f>'Burndown Chart'!B7*0.75</f>
-        <v>16.5</v>
+        <f>'Burndown Chart'!B7</f>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
@@ -2259,7 +2296,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2271,11 +2308,11 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <f>'Burndown Chart'!B7/4</f>
-        <v>5.5</v>
+        <f>'Burndown Chart'!B13</f>
+        <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2335,7 +2372,7 @@
         <v>62</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2395,7 +2432,7 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2441,7 +2478,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2481,7 +2518,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2564,7 +2601,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2584,7 +2621,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2655,7 +2692,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
         <v>29</v>
@@ -2675,7 +2712,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D8" t="s">
         <v>29</v>
@@ -2695,7 +2732,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
@@ -2801,7 +2838,7 @@
         <v>50</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -2841,13 +2878,13 @@
         <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2918,7 +2955,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" t="s">
         <v>27</v>
@@ -2927,7 +2964,7 @@
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -2940,7 +2977,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3024,7 +3061,7 @@
         <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -3124,7 +3161,7 @@
         <v>59</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9">
         <v>5</v>
@@ -3150,7 +3187,7 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -3160,10 +3197,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3204,7 +3241,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
@@ -3214,6 +3251,86 @@
       </c>
       <c r="F2" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated scrum and some of the reviews
</commit_message>
<xml_diff>
--- a/Documentation/Scrum.xlsx
+++ b/Documentation/Scrum.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="87">
   <si>
     <t>Actual remaining hours</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Façade design pattern</t>
   </si>
   <si>
-    <t>Remote observer d.p.</t>
-  </si>
-  <si>
     <t>MVC design pattern</t>
   </si>
   <si>
@@ -234,9 +231,6 @@
     <t>All</t>
   </si>
   <si>
-    <t>Not done</t>
-  </si>
-  <si>
     <t>In progress</t>
   </si>
   <si>
@@ -292,6 +286,18 @@
   </si>
   <si>
     <t>Finnish MVC documentation</t>
+  </si>
+  <si>
+    <t>Observer design pattern</t>
+  </si>
+  <si>
+    <t>Customer wants clean code without redundant methods and useless sysouts.</t>
+  </si>
+  <si>
+    <t>Clean code</t>
+  </si>
+  <si>
+    <t>Delete reduntant methods and sysouts, clean code</t>
   </si>
 </sst>
 </file>
@@ -499,7 +505,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$A$15</c:f>
+              <c:f>'Burndown Chart'!$A$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -560,33 +566,33 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$15:$I$15</c:f>
+              <c:f>'Burndown Chart'!$B$16:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>68</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67</c:v>
+                  <c:v>69</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57</c:v>
+                  <c:v>59</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>27</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -603,7 +609,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Burndown Chart'!$A$16</c:f>
+              <c:f>'Burndown Chart'!$A$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -664,30 +670,30 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burndown Chart'!$B$16:$I$16</c:f>
+              <c:f>'Burndown Chart'!$B$17:$I$17</c:f>
               <c:numCache>
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>68</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>58.285714285714285</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>48.571428571428569</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.857142857142854</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.142857142857139</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.428571428571423</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.71428571428571</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1447,13 +1453,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>857249</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1779,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,13 +1850,13 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
       <c r="J2" s="5">
-        <f t="shared" ref="J2:J13" si="0">SUM(C2:I2)</f>
+        <f t="shared" ref="J2:J14" si="0">SUM(C2:I2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B3" s="5">
         <v>2</v>
@@ -1892,7 +1898,7 @@
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="5">
         <v>5</v>
@@ -1913,7 +1919,7 @@
     </row>
     <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B6" s="5">
         <v>5</v>
@@ -1934,7 +1940,7 @@
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="B7" s="5">
         <v>18</v>
@@ -1955,7 +1961,7 @@
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="5">
         <v>9</v>
@@ -1995,7 +2001,7 @@
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B10" s="5">
         <v>3</v>
@@ -2003,18 +2009,20 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="F10" s="6">
+        <v>3</v>
+      </c>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B11" s="5">
         <v>5</v>
@@ -2035,7 +2043,7 @@
     </row>
     <row r="12" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B12" s="5">
         <v>3</v>
@@ -2056,7 +2064,7 @@
     </row>
     <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B13" s="5">
         <v>4</v>
@@ -2065,93 +2073,114 @@
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
+      <c r="G13" s="6">
+        <v>4</v>
+      </c>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="5">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="5">
+        <v>2</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="5">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="J14" s="6"/>
-    </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="5">
-        <f>SUM(B2:B13)</f>
-        <v>68</v>
-      </c>
-      <c r="C15" s="5">
-        <f>B15-(SUM(C2:C13))</f>
-        <v>67</v>
-      </c>
-      <c r="D15" s="5">
-        <f t="shared" ref="D15:I15" si="1">C15-(SUM(D2:D13))</f>
-        <v>57</v>
-      </c>
-      <c r="E15" s="5">
+      <c r="B16" s="5">
+        <f>SUM(B2:B14)</f>
+        <v>70</v>
+      </c>
+      <c r="C16" s="5">
+        <f>B16-(SUM(C2:C14))</f>
+        <v>69</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" ref="D16:I16" si="1">C16-(SUM(D2:D14))</f>
+        <v>59</v>
+      </c>
+      <c r="E16" s="5">
         <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="F16" s="5">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="G16" s="5">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I16" s="5">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5">
+        <f>SUM(B2:B14)</f>
+        <v>70</v>
+      </c>
+      <c r="C17" s="7">
+        <f>B17-($B$17/7)</f>
+        <v>60</v>
+      </c>
+      <c r="D17" s="7">
+        <f t="shared" ref="D17:I17" si="2">C17-($B$17/7)</f>
         <v>50</v>
       </c>
-      <c r="F15" s="5">
-        <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="G15" s="5">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="H15" s="5">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-      <c r="I15" s="5">
-        <f t="shared" si="1"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="5">
-        <f>SUM(B2:B13)</f>
-        <v>68</v>
-      </c>
-      <c r="C16" s="7">
-        <f>B16-($B$16/7)</f>
-        <v>58.285714285714285</v>
-      </c>
-      <c r="D16" s="7">
-        <f t="shared" ref="D16:I16" si="2">C16-($B$16/7)</f>
-        <v>48.571428571428569</v>
-      </c>
-      <c r="E16" s="7">
+      <c r="E17" s="7">
         <f t="shared" si="2"/>
-        <v>38.857142857142854</v>
-      </c>
-      <c r="F16" s="7">
+        <v>40</v>
+      </c>
+      <c r="F17" s="7">
         <f t="shared" si="2"/>
-        <v>29.142857142857139</v>
-      </c>
-      <c r="G16" s="7">
+        <v>30</v>
+      </c>
+      <c r="G17" s="7">
         <f t="shared" si="2"/>
-        <v>19.428571428571423</v>
-      </c>
-      <c r="H16" s="7">
+        <v>20</v>
+      </c>
+      <c r="H17" s="7">
         <f t="shared" si="2"/>
-        <v>9.71428571428571</v>
-      </c>
-      <c r="I16" s="7">
+        <v>10</v>
+      </c>
+      <c r="I17" s="7">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="8" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:9" s="8" customFormat="1" ht="2.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2161,10 +2190,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2189,11 +2218,11 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f t="shared" ref="A3:A14" si="0">A2+1</f>
+        <f t="shared" ref="A3:A15" si="0">A2+1</f>
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3">
         <f>'Burndown Chart'!B2</f>
@@ -2209,14 +2238,14 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4">
         <f>'Burndown Chart'!B3</f>
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2225,14 +2254,14 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <f>'Burndown Chart'!B7</f>
         <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2241,14 +2270,14 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <f>'Burndown Chart'!B6</f>
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2257,14 +2286,14 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C7">
         <f>'Burndown Chart'!B5</f>
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2273,14 +2302,14 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
         <f>'Burndown Chart'!B4</f>
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2289,14 +2318,14 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9">
         <f>'Burndown Chart'!B11</f>
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2305,14 +2334,14 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <f>'Burndown Chart'!B13</f>
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2321,14 +2350,14 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <f>'Burndown Chart'!B8</f>
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2337,14 +2366,14 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12">
         <f>'Burndown Chart'!B9</f>
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -2353,7 +2382,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C13">
         <f>'Burndown Chart'!B12</f>
@@ -2369,10 +2398,30 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="C14">
+        <f>'Burndown Chart'!B10</f>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15">
+        <f>'Burndown Chart'!B14</f>
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -2403,22 +2452,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2429,16 +2478,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2449,16 +2498,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2469,16 +2518,16 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2489,16 +2538,16 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2509,16 +2558,16 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2529,16 +2578,16 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2551,7 +2600,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:F9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2566,22 +2615,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2592,16 +2641,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2612,16 +2661,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2632,16 +2681,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2652,16 +2701,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2672,16 +2721,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2692,16 +2741,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2712,16 +2761,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2732,16 +2781,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2754,7 +2803,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E16" sqref="E16:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2769,22 +2818,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2795,16 +2844,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>7</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2815,16 +2864,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2835,16 +2884,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E4">
         <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2855,16 +2904,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2875,16 +2924,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E6">
         <v>3</v>
       </c>
       <c r="F6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2895,16 +2944,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2915,16 +2964,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2935,16 +2984,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2955,16 +3004,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -2977,7 +3026,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2992,22 +3041,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3018,16 +3067,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3038,16 +3087,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3058,16 +3107,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3078,16 +3127,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3098,16 +3147,16 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -3118,16 +3167,16 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -3138,16 +3187,16 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -3158,16 +3207,16 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E9">
         <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -3178,16 +3227,16 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10">
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -3197,10 +3246,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3215,22 +3264,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
       </c>
       <c r="E1" t="s">
         <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -3241,16 +3290,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3261,16 +3310,16 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3281,16 +3330,16 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -3301,16 +3350,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -3321,16 +3370,36 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>81</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>13</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>